<commit_message>
Atualização de agendamento/ Adicionado campos do agendamento nos Casos de Uso
</commit_message>
<xml_diff>
--- a/Casos de uso.xlsx
+++ b/Casos de uso.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isac\Desktop\Faculdade\pim\1-2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Documents\GitHub\Enfermagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E195AC-8D37-46DA-95DE-3E97C7F13C14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE9F077-1D7D-49AC-910C-BBAC94B02D2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6BB21F3B-7A02-4EF4-A239-0FC69613A7E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>CASOS DE USO</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Atores:</t>
-  </si>
-  <si>
     <t>Coordenador, Eferemeiro, Professor Auxiliar, Alunos</t>
   </si>
   <si>
@@ -48,27 +45,15 @@
     <t>Com o usuário e senha previamente cadastradas, o ator deverá colocá-los nos lugares indicados e assim acessar o sistema</t>
   </si>
   <si>
-    <t>ATOR ESPERA:</t>
-  </si>
-  <si>
     <t>DESCRIÇÃO</t>
   </si>
   <si>
-    <t>ERRO:</t>
-  </si>
-  <si>
     <t>Usuário esqueceu a senha (no caso senha inválida), ou ele já está inativo ou ainda não foi cadastrado</t>
   </si>
   <si>
-    <t>ALTERNATIVA:</t>
-  </si>
-  <si>
     <t>Entrar em contato com o coordenador para efetuar seu cadastro ou trocar sua senha</t>
   </si>
   <si>
-    <t>FINAL:</t>
-  </si>
-  <si>
     <t>Usuário acessa o sistema</t>
   </si>
   <si>
@@ -142,6 +127,57 @@
   </si>
   <si>
     <t>Exibir as informações dos paciente desejado</t>
+  </si>
+  <si>
+    <t>Agendar consulta</t>
+  </si>
+  <si>
+    <t>Coordenador, Enfermeiro, Professor Auxiliar, Alunos</t>
+  </si>
+  <si>
+    <t>Realizar agendamento de consultas futuras</t>
+  </si>
+  <si>
+    <t>Selecionar próxima data e horário disponível/Cadastrar Paciente</t>
+  </si>
+  <si>
+    <t>A data e horário selecionada já possui consulta ou paciente não cadastrado</t>
+  </si>
+  <si>
+    <t>Os atores irão preencher os campos informados e selecionar a data e horário para agendamento</t>
+  </si>
+  <si>
+    <t>Consulta cadastrada com sucesso</t>
+  </si>
+  <si>
+    <t>ATORES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOME DO CASO </t>
+  </si>
+  <si>
+    <t>ATOR ESPERA</t>
+  </si>
+  <si>
+    <t>ERRO</t>
+  </si>
+  <si>
+    <t>ALTERNATIVA</t>
+  </si>
+  <si>
+    <t>FINAL</t>
+  </si>
+  <si>
+    <t>Vizualizar agendamento</t>
+  </si>
+  <si>
+    <t>Vizualizar as futuras consultas pendentes</t>
+  </si>
+  <si>
+    <t>Os atores irão visualizar os devidos horários e datas das consultas futuras dos pacientes e pesquisar por dias específicos</t>
+  </si>
+  <si>
+    <t>As informações de agendamento exibidas</t>
   </si>
 </sst>
 </file>
@@ -206,11 +242,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,14 +260,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA21ED-9240-46D0-9631-45BE1952D415}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,319 +597,441 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
+      <c r="A3" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="B51" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>38</v>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>